<commit_message>
changes in the summary table
</commit_message>
<xml_diff>
--- a/media/summary_output.xlsx
+++ b/media/summary_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="24">
   <si>
     <t>Service Type Offered</t>
   </si>
@@ -31,13 +31,22 @@
     <t>Total_Spend</t>
   </si>
   <si>
+    <t>Spend %</t>
+  </si>
+  <si>
     <t>Base_Rate</t>
+  </si>
+  <si>
+    <t>Base Rate %</t>
   </si>
   <si>
     <t>Total_Accessorial</t>
   </si>
   <si>
-    <t>Disc</t>
+    <t>Accessorial %</t>
+  </si>
+  <si>
+    <t>Max Disc</t>
   </si>
   <si>
     <t>Client's Min</t>
@@ -434,13 +443,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,13 +477,22 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -486,24 +504,33 @@
         <v>202.45</v>
       </c>
       <c r="F2">
+        <v>0.4</v>
+      </c>
+      <c r="G2">
         <v>90.81999999999999</v>
       </c>
-      <c r="G2">
+      <c r="H2">
+        <v>44.86</v>
+      </c>
+      <c r="I2">
         <v>111.63</v>
       </c>
-      <c r="H2">
+      <c r="J2">
+        <v>55.14</v>
+      </c>
+      <c r="K2">
         <v>56.99</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -515,24 +542,33 @@
         <v>871.12</v>
       </c>
       <c r="F3">
+        <v>1.73</v>
+      </c>
+      <c r="G3">
         <v>371.31</v>
       </c>
-      <c r="G3">
+      <c r="H3">
+        <v>42.62</v>
+      </c>
+      <c r="I3">
         <v>499.81</v>
       </c>
-      <c r="H3">
+      <c r="J3">
+        <v>57.38</v>
+      </c>
+      <c r="K3">
         <v>61.82</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -544,24 +580,33 @@
         <v>2572.97</v>
       </c>
       <c r="F4">
+        <v>5.12</v>
+      </c>
+      <c r="G4">
         <v>1118.81</v>
       </c>
-      <c r="G4">
+      <c r="H4">
+        <v>43.48</v>
+      </c>
+      <c r="I4">
         <v>1454.16</v>
       </c>
-      <c r="H4">
+      <c r="J4">
+        <v>56.52</v>
+      </c>
+      <c r="K4">
         <v>61.58</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -573,24 +618,33 @@
         <v>2351.38</v>
       </c>
       <c r="F5">
+        <v>4.68</v>
+      </c>
+      <c r="G5">
         <v>1046.68</v>
       </c>
-      <c r="G5">
+      <c r="H5">
+        <v>44.51</v>
+      </c>
+      <c r="I5">
         <v>1304.7</v>
       </c>
-      <c r="H5">
+      <c r="J5">
+        <v>55.49</v>
+      </c>
+      <c r="K5">
         <v>67.89</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -602,24 +656,33 @@
         <v>34.92</v>
       </c>
       <c r="F6">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G6">
         <v>21.17</v>
       </c>
-      <c r="G6">
+      <c r="H6">
+        <v>60.62</v>
+      </c>
+      <c r="I6">
         <v>13.75</v>
       </c>
-      <c r="H6">
+      <c r="J6">
+        <v>39.38</v>
+      </c>
+      <c r="K6">
         <v>62</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -631,24 +694,33 @@
         <v>990.1899999999999</v>
       </c>
       <c r="F7">
+        <v>1.97</v>
+      </c>
+      <c r="G7">
         <v>504.48</v>
       </c>
-      <c r="G7">
+      <c r="H7">
+        <v>50.95</v>
+      </c>
+      <c r="I7">
         <v>485.71</v>
       </c>
-      <c r="H7">
+      <c r="J7">
+        <v>49.05</v>
+      </c>
+      <c r="K7">
         <v>78.64</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -660,24 +732,33 @@
         <v>1064.15</v>
       </c>
       <c r="F8">
+        <v>2.12</v>
+      </c>
+      <c r="G8">
         <v>545.3</v>
       </c>
-      <c r="G8">
+      <c r="H8">
+        <v>51.24</v>
+      </c>
+      <c r="I8">
         <v>518.85</v>
       </c>
-      <c r="H8">
+      <c r="J8">
+        <v>48.76</v>
+      </c>
+      <c r="K8">
         <v>75.44</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -689,24 +770,33 @@
         <v>22.07</v>
       </c>
       <c r="F9">
+        <v>0.04</v>
+      </c>
+      <c r="G9">
         <v>13.95</v>
       </c>
-      <c r="G9">
+      <c r="H9">
+        <v>63.21</v>
+      </c>
+      <c r="I9">
         <v>8.119999999999999</v>
       </c>
-      <c r="H9">
+      <c r="J9">
+        <v>36.79</v>
+      </c>
+      <c r="K9">
         <v>59.99</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -718,24 +808,33 @@
         <v>75.69</v>
       </c>
       <c r="F10">
+        <v>0.15</v>
+      </c>
+      <c r="G10">
         <v>48.16</v>
       </c>
-      <c r="G10">
+      <c r="H10">
+        <v>63.63</v>
+      </c>
+      <c r="I10">
         <v>27.53</v>
       </c>
-      <c r="H10">
+      <c r="J10">
+        <v>36.37</v>
+      </c>
+      <c r="K10">
         <v>60.01</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -747,24 +846,33 @@
         <v>95.28</v>
       </c>
       <c r="F11">
+        <v>0.19</v>
+      </c>
+      <c r="G11">
         <v>67.98</v>
       </c>
-      <c r="G11">
+      <c r="H11">
+        <v>71.34999999999999</v>
+      </c>
+      <c r="I11">
         <v>27.3</v>
       </c>
-      <c r="H11">
+      <c r="J11">
+        <v>28.65</v>
+      </c>
+      <c r="K11">
         <v>64.01000000000001</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>6</v>
@@ -776,24 +884,33 @@
         <v>147.56</v>
       </c>
       <c r="F12">
+        <v>0.29</v>
+      </c>
+      <c r="G12">
         <v>60.78</v>
       </c>
-      <c r="G12">
+      <c r="H12">
+        <v>41.19</v>
+      </c>
+      <c r="I12">
         <v>86.78</v>
       </c>
-      <c r="H12">
+      <c r="J12">
+        <v>58.81</v>
+      </c>
+      <c r="K12">
         <v>64</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -805,24 +922,33 @@
         <v>35.6</v>
       </c>
       <c r="F13">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G13">
         <v>13.68</v>
       </c>
-      <c r="G13">
+      <c r="H13">
+        <v>38.43</v>
+      </c>
+      <c r="I13">
         <v>21.92</v>
       </c>
-      <c r="H13">
+      <c r="J13">
+        <v>61.57</v>
+      </c>
+      <c r="K13">
         <v>56.98</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -834,24 +960,33 @@
         <v>62.41</v>
       </c>
       <c r="F14">
+        <v>0.12</v>
+      </c>
+      <c r="G14">
         <v>25.68</v>
       </c>
-      <c r="G14">
+      <c r="H14">
+        <v>41.15</v>
+      </c>
+      <c r="I14">
         <v>36.73</v>
       </c>
-      <c r="H14">
+      <c r="J14">
+        <v>58.85</v>
+      </c>
+      <c r="K14">
         <v>57</v>
       </c>
-      <c r="I14">
+      <c r="L14">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -863,24 +998,33 @@
         <v>118.81</v>
       </c>
       <c r="F15">
+        <v>0.24</v>
+      </c>
+      <c r="G15">
         <v>51.11</v>
       </c>
-      <c r="G15">
+      <c r="H15">
+        <v>43.02</v>
+      </c>
+      <c r="I15">
         <v>67.7</v>
       </c>
-      <c r="H15">
+      <c r="J15">
+        <v>56.98</v>
+      </c>
+      <c r="K15">
         <v>57.02</v>
       </c>
-      <c r="I15">
+      <c r="L15">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -892,24 +1036,33 @@
         <v>148.8</v>
       </c>
       <c r="F16">
+        <v>0.3</v>
+      </c>
+      <c r="G16">
         <v>61.73</v>
       </c>
-      <c r="G16">
+      <c r="H16">
+        <v>41.49</v>
+      </c>
+      <c r="I16">
         <v>87.06999999999999</v>
       </c>
-      <c r="H16">
+      <c r="J16">
+        <v>58.51</v>
+      </c>
+      <c r="K16">
         <v>62</v>
       </c>
-      <c r="I16">
+      <c r="L16">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -921,24 +1074,33 @@
         <v>472.8</v>
       </c>
       <c r="F17">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="G17">
         <v>222.47</v>
       </c>
-      <c r="G17">
+      <c r="H17">
+        <v>47.05</v>
+      </c>
+      <c r="I17">
         <v>250.33</v>
       </c>
-      <c r="H17">
+      <c r="J17">
+        <v>52.95</v>
+      </c>
+      <c r="K17">
         <v>57</v>
       </c>
-      <c r="I17">
+      <c r="L17">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -950,24 +1112,33 @@
         <v>1627.12</v>
       </c>
       <c r="F18">
+        <v>3.24</v>
+      </c>
+      <c r="G18">
         <v>770.33</v>
       </c>
-      <c r="G18">
+      <c r="H18">
+        <v>47.34</v>
+      </c>
+      <c r="I18">
         <v>856.79</v>
       </c>
-      <c r="H18">
+      <c r="J18">
+        <v>52.66</v>
+      </c>
+      <c r="K18">
         <v>58.97</v>
       </c>
-      <c r="I18">
+      <c r="L18">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -979,24 +1150,33 @@
         <v>3338.24</v>
       </c>
       <c r="F19">
+        <v>6.65</v>
+      </c>
+      <c r="G19">
         <v>1628.83</v>
       </c>
-      <c r="G19">
+      <c r="H19">
+        <v>48.79</v>
+      </c>
+      <c r="I19">
         <v>1709.41</v>
       </c>
-      <c r="H19">
+      <c r="J19">
+        <v>51.21</v>
+      </c>
+      <c r="K19">
         <v>60.53</v>
       </c>
-      <c r="I19">
+      <c r="L19">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -1008,24 +1188,33 @@
         <v>2537.73</v>
       </c>
       <c r="F20">
+        <v>5.05</v>
+      </c>
+      <c r="G20">
         <v>1230.18</v>
       </c>
-      <c r="G20">
+      <c r="H20">
+        <v>48.48</v>
+      </c>
+      <c r="I20">
         <v>1307.55</v>
       </c>
-      <c r="H20">
+      <c r="J20">
+        <v>51.52</v>
+      </c>
+      <c r="K20">
         <v>67.48</v>
       </c>
-      <c r="I20">
+      <c r="L20">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>6</v>
@@ -1037,24 +1226,33 @@
         <v>341</v>
       </c>
       <c r="F21">
+        <v>0.68</v>
+      </c>
+      <c r="G21">
         <v>185.73</v>
       </c>
-      <c r="G21">
+      <c r="H21">
+        <v>54.47</v>
+      </c>
+      <c r="I21">
         <v>155.27</v>
       </c>
-      <c r="H21">
+      <c r="J21">
+        <v>45.53</v>
+      </c>
+      <c r="K21">
         <v>71.05</v>
       </c>
-      <c r="I21">
+      <c r="L21">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>7</v>
@@ -1066,24 +1264,33 @@
         <v>519.29</v>
       </c>
       <c r="F22">
+        <v>1.03</v>
+      </c>
+      <c r="G22">
         <v>316.26</v>
       </c>
-      <c r="G22">
+      <c r="H22">
+        <v>60.9</v>
+      </c>
+      <c r="I22">
         <v>203.03</v>
       </c>
-      <c r="H22">
+      <c r="J22">
+        <v>39.1</v>
+      </c>
+      <c r="K22">
         <v>72.45999999999999</v>
       </c>
-      <c r="I22">
+      <c r="L22">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C23">
         <v>8</v>
@@ -1095,24 +1302,33 @@
         <v>365.84</v>
       </c>
       <c r="F23">
+        <v>0.73</v>
+      </c>
+      <c r="G23">
         <v>196.4</v>
       </c>
-      <c r="G23">
+      <c r="H23">
+        <v>53.68</v>
+      </c>
+      <c r="I23">
         <v>169.44</v>
       </c>
-      <c r="H23">
+      <c r="J23">
+        <v>46.32</v>
+      </c>
+      <c r="K23">
         <v>75.19</v>
       </c>
-      <c r="I23">
+      <c r="L23">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1124,24 +1340,33 @@
         <v>49.2</v>
       </c>
       <c r="F24">
+        <v>0.1</v>
+      </c>
+      <c r="G24">
         <v>37.33</v>
       </c>
-      <c r="G24">
+      <c r="H24">
+        <v>75.87</v>
+      </c>
+      <c r="I24">
         <v>11.87</v>
       </c>
-      <c r="H24">
+      <c r="J24">
+        <v>24.13</v>
+      </c>
+      <c r="K24">
         <v>63.99</v>
       </c>
-      <c r="I24">
+      <c r="L24">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -1153,24 +1378,33 @@
         <v>50.73</v>
       </c>
       <c r="F25">
+        <v>0.1</v>
+      </c>
+      <c r="G25">
         <v>23.71</v>
       </c>
-      <c r="G25">
+      <c r="H25">
+        <v>46.74</v>
+      </c>
+      <c r="I25">
         <v>27.02</v>
       </c>
-      <c r="H25">
+      <c r="J25">
+        <v>53.26</v>
+      </c>
+      <c r="K25">
         <v>57.01</v>
       </c>
-      <c r="I25">
+      <c r="L25">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1182,24 +1416,33 @@
         <v>28.39</v>
       </c>
       <c r="F26">
+        <v>0.06</v>
+      </c>
+      <c r="G26">
         <v>12.46</v>
       </c>
-      <c r="G26">
+      <c r="H26">
+        <v>43.89</v>
+      </c>
+      <c r="I26">
         <v>15.93</v>
       </c>
-      <c r="H26">
+      <c r="J26">
+        <v>56.11</v>
+      </c>
+      <c r="K26">
         <v>57</v>
       </c>
-      <c r="I26">
+      <c r="L26">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C27">
         <v>8</v>
@@ -1211,24 +1454,33 @@
         <v>49.47</v>
       </c>
       <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="G27">
         <v>37.57</v>
       </c>
-      <c r="G27">
+      <c r="H27">
+        <v>75.95</v>
+      </c>
+      <c r="I27">
         <v>11.9</v>
       </c>
-      <c r="H27">
+      <c r="J27">
+        <v>24.05</v>
+      </c>
+      <c r="K27">
         <v>62</v>
       </c>
-      <c r="I27">
+      <c r="L27">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1240,21 +1492,30 @@
         <v>982.3</v>
       </c>
       <c r="F28">
+        <v>1.96</v>
+      </c>
+      <c r="G28">
         <v>838.3</v>
       </c>
-      <c r="G28">
+      <c r="H28">
+        <v>85.34</v>
+      </c>
+      <c r="I28">
         <v>144</v>
       </c>
-      <c r="I28">
+      <c r="J28">
+        <v>14.66</v>
+      </c>
+      <c r="L28">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1266,21 +1527,30 @@
         <v>3403.05</v>
       </c>
       <c r="F29">
+        <v>6.78</v>
+      </c>
+      <c r="G29">
         <v>2955.33</v>
       </c>
-      <c r="G29">
+      <c r="H29">
+        <v>86.84</v>
+      </c>
+      <c r="I29">
         <v>447.72</v>
       </c>
-      <c r="I29">
+      <c r="J29">
+        <v>13.16</v>
+      </c>
+      <c r="L29">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -1292,21 +1562,30 @@
         <v>9748.679999999998</v>
       </c>
       <c r="F30">
+        <v>19.41</v>
+      </c>
+      <c r="G30">
         <v>8359.019999999999</v>
       </c>
-      <c r="G30">
+      <c r="H30">
+        <v>85.75</v>
+      </c>
+      <c r="I30">
         <v>1389.66</v>
       </c>
-      <c r="I30">
+      <c r="J30">
+        <v>14.25</v>
+      </c>
+      <c r="L30">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -1318,21 +1597,30 @@
         <v>7936.08</v>
       </c>
       <c r="F31">
+        <v>15.8</v>
+      </c>
+      <c r="G31">
         <v>6753.169999999999</v>
       </c>
-      <c r="G31">
+      <c r="H31">
+        <v>85.09</v>
+      </c>
+      <c r="I31">
         <v>1182.91</v>
       </c>
-      <c r="I31">
+      <c r="J31">
+        <v>14.91</v>
+      </c>
+      <c r="L31">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>6</v>
@@ -1344,21 +1632,30 @@
         <v>1119.7</v>
       </c>
       <c r="F32">
+        <v>2.23</v>
+      </c>
+      <c r="G32">
         <v>951.6999999999999</v>
       </c>
-      <c r="G32">
+      <c r="H32">
+        <v>85</v>
+      </c>
+      <c r="I32">
         <v>168</v>
       </c>
-      <c r="I32">
+      <c r="J32">
+        <v>15</v>
+      </c>
+      <c r="L32">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>7</v>
@@ -1370,21 +1667,30 @@
         <v>3604.95</v>
       </c>
       <c r="F33">
+        <v>7.18</v>
+      </c>
+      <c r="G33">
         <v>3064.89</v>
       </c>
-      <c r="G33">
+      <c r="H33">
+        <v>85.02</v>
+      </c>
+      <c r="I33">
         <v>540.0599999999999</v>
       </c>
-      <c r="I33">
+      <c r="J33">
+        <v>14.98</v>
+      </c>
+      <c r="L33">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C34">
         <v>8</v>
@@ -1396,21 +1702,30 @@
         <v>2317.66</v>
       </c>
       <c r="F34">
+        <v>4.61</v>
+      </c>
+      <c r="G34">
         <v>1997.09</v>
       </c>
-      <c r="G34">
+      <c r="H34">
+        <v>86.17</v>
+      </c>
+      <c r="I34">
         <v>320.57</v>
       </c>
-      <c r="I34">
+      <c r="J34">
+        <v>13.83</v>
+      </c>
+      <c r="L34">
         <v>9.199999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -1422,24 +1737,33 @@
         <v>13.46</v>
       </c>
       <c r="F35">
-        <v>10.7</v>
+        <v>0.03</v>
       </c>
       <c r="G35">
+        <v>10.7</v>
+      </c>
+      <c r="H35">
+        <v>79.48999999999999</v>
+      </c>
+      <c r="I35">
         <v>2.76</v>
       </c>
-      <c r="H35">
+      <c r="J35">
+        <v>20.51</v>
+      </c>
+      <c r="K35">
         <v>10.83</v>
       </c>
-      <c r="I35">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="L35">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -1451,24 +1775,33 @@
         <v>79.36</v>
       </c>
       <c r="F36">
+        <v>0.16</v>
+      </c>
+      <c r="G36">
         <v>53.5</v>
       </c>
-      <c r="G36">
+      <c r="H36">
+        <v>67.41</v>
+      </c>
+      <c r="I36">
         <v>25.86</v>
       </c>
-      <c r="H36">
+      <c r="J36">
+        <v>32.59</v>
+      </c>
+      <c r="K36">
         <v>20.03</v>
       </c>
-      <c r="I36">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="L36">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -1480,24 +1813,33 @@
         <v>143.05</v>
       </c>
       <c r="F37">
+        <v>0.28</v>
+      </c>
+      <c r="G37">
         <v>85.59999999999999</v>
       </c>
-      <c r="G37">
+      <c r="H37">
+        <v>59.84</v>
+      </c>
+      <c r="I37">
         <v>53.45</v>
       </c>
-      <c r="H37">
+      <c r="J37">
+        <v>37.36</v>
+      </c>
+      <c r="K37">
         <v>29.19</v>
       </c>
-      <c r="I37">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="L37">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -1509,24 +1851,33 @@
         <v>222.4</v>
       </c>
       <c r="F38">
+        <v>0.44</v>
+      </c>
+      <c r="G38">
         <v>128.4</v>
       </c>
-      <c r="G38">
+      <c r="H38">
+        <v>57.73</v>
+      </c>
+      <c r="I38">
         <v>94</v>
       </c>
-      <c r="H38">
+      <c r="J38">
+        <v>42.27</v>
+      </c>
+      <c r="K38">
         <v>35.7</v>
       </c>
-      <c r="I38">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="L38">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -1538,24 +1889,33 @@
         <v>26.92</v>
       </c>
       <c r="F39">
+        <v>0.05</v>
+      </c>
+      <c r="G39">
         <v>21.4</v>
       </c>
-      <c r="G39">
+      <c r="H39">
+        <v>79.48999999999999</v>
+      </c>
+      <c r="I39">
         <v>5.52</v>
       </c>
-      <c r="H39">
+      <c r="J39">
+        <v>20.51</v>
+      </c>
+      <c r="K39">
         <v>17.69</v>
       </c>
-      <c r="I39">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="L39">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C40">
         <v>7</v>
@@ -1567,24 +1927,33 @@
         <v>53.76000000000001</v>
       </c>
       <c r="F40">
+        <v>0.11</v>
+      </c>
+      <c r="G40">
         <v>32.09999999999999</v>
       </c>
-      <c r="G40">
+      <c r="H40">
+        <v>59.71</v>
+      </c>
+      <c r="I40">
         <v>21.66</v>
       </c>
-      <c r="H40">
+      <c r="J40">
+        <v>40.29</v>
+      </c>
+      <c r="K40">
         <v>38.65</v>
       </c>
-      <c r="I40">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="L40">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C41">
         <v>8</v>
@@ -1596,24 +1965,33 @@
         <v>75.63</v>
       </c>
       <c r="F41">
+        <v>0.15</v>
+      </c>
+      <c r="G41">
         <v>43.04</v>
       </c>
-      <c r="G41">
+      <c r="H41">
+        <v>56.91</v>
+      </c>
+      <c r="I41">
         <v>32.59</v>
       </c>
-      <c r="H41">
+      <c r="J41">
+        <v>43.09</v>
+      </c>
+      <c r="K41">
         <v>43.98</v>
       </c>
-      <c r="I41">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="L41">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C42">
         <v>5</v>
@@ -1625,24 +2003,33 @@
         <v>44.59</v>
       </c>
       <c r="F42">
+        <v>0.09</v>
+      </c>
+      <c r="G42">
         <v>32.34</v>
       </c>
-      <c r="G42">
+      <c r="H42">
+        <v>72.53</v>
+      </c>
+      <c r="I42">
         <v>12.25</v>
       </c>
-      <c r="H42">
+      <c r="J42">
+        <v>27.47</v>
+      </c>
+      <c r="K42">
         <v>47.98</v>
       </c>
-      <c r="I42">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="L42">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C43">
         <v>8</v>
@@ -1654,24 +2041,33 @@
         <v>32.57</v>
       </c>
       <c r="F43">
+        <v>0.06</v>
+      </c>
+      <c r="G43">
         <v>14.28</v>
       </c>
-      <c r="G43">
+      <c r="H43">
+        <v>43.84</v>
+      </c>
+      <c r="I43">
         <v>18.29</v>
       </c>
-      <c r="H43">
+      <c r="J43">
+        <v>56.16</v>
+      </c>
+      <c r="K43">
         <v>48.02</v>
       </c>
-      <c r="I43">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="L43">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C44">
         <v>4</v>
@@ -1683,24 +2079,33 @@
         <v>57.65</v>
       </c>
       <c r="F44">
+        <v>0.11</v>
+      </c>
+      <c r="G44">
         <v>49.7</v>
       </c>
-      <c r="G44">
+      <c r="H44">
+        <v>86.20999999999999</v>
+      </c>
+      <c r="I44">
         <v>7.949999999999999</v>
       </c>
-      <c r="H44">
+      <c r="J44">
+        <v>13.79</v>
+      </c>
+      <c r="K44">
         <v>49.01</v>
       </c>
-      <c r="I44">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="L44">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C45">
         <v>8</v>
@@ -1712,24 +2117,33 @@
         <v>64.67</v>
       </c>
       <c r="F45">
+        <v>0.13</v>
+      </c>
+      <c r="G45">
         <v>44.75</v>
       </c>
-      <c r="G45">
+      <c r="H45">
+        <v>69.2</v>
+      </c>
+      <c r="I45">
         <v>19.92</v>
       </c>
-      <c r="H45">
+      <c r="J45">
+        <v>30.8</v>
+      </c>
+      <c r="K45">
         <v>48.99</v>
       </c>
-      <c r="I45">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="L45">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C46">
         <v>4</v>
@@ -1741,24 +2155,33 @@
         <v>35.28</v>
       </c>
       <c r="F46">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G46">
         <v>30.41</v>
       </c>
-      <c r="G46">
+      <c r="H46">
+        <v>86.2</v>
+      </c>
+      <c r="I46">
         <v>4.87</v>
       </c>
-      <c r="H46">
+      <c r="J46">
+        <v>13.8</v>
+      </c>
+      <c r="K46">
         <v>52.01</v>
       </c>
-      <c r="I46">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="L46">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C47">
         <v>8</v>
@@ -1770,24 +2193,33 @@
         <v>31.47</v>
       </c>
       <c r="F47">
+        <v>0.06</v>
+      </c>
+      <c r="G47">
         <v>27.13</v>
       </c>
-      <c r="G47">
+      <c r="H47">
+        <v>86.20999999999999</v>
+      </c>
+      <c r="I47">
         <v>4.34</v>
       </c>
-      <c r="H47">
+      <c r="J47">
+        <v>13.79</v>
+      </c>
+      <c r="K47">
         <v>52.01</v>
       </c>
-      <c r="I47">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="L47">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -1799,24 +2231,33 @@
         <v>47.91</v>
       </c>
       <c r="F48">
+        <v>0.1</v>
+      </c>
+      <c r="G48">
         <v>21.4</v>
       </c>
-      <c r="G48">
+      <c r="H48">
+        <v>44.67</v>
+      </c>
+      <c r="I48">
         <v>26.51</v>
       </c>
-      <c r="H48">
+      <c r="J48">
+        <v>55.33</v>
+      </c>
+      <c r="K48">
         <v>23.41</v>
       </c>
-      <c r="I48">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="L48">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C49">
         <v>3</v>
@@ -1828,24 +2269,33 @@
         <v>65.08</v>
       </c>
       <c r="F49">
+        <v>0.13</v>
+      </c>
+      <c r="G49">
         <v>32.09999999999999</v>
       </c>
-      <c r="G49">
+      <c r="H49">
+        <v>49.32</v>
+      </c>
+      <c r="I49">
         <v>32.98</v>
       </c>
-      <c r="H49">
+      <c r="J49">
+        <v>50.68</v>
+      </c>
+      <c r="K49">
         <v>28.9</v>
       </c>
-      <c r="I49">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="L49">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C50">
         <v>4</v>
@@ -1857,24 +2307,33 @@
         <v>148.95</v>
       </c>
       <c r="F50">
+        <v>0.3</v>
+      </c>
+      <c r="G50">
         <v>85.59999999999999</v>
       </c>
-      <c r="G50">
+      <c r="H50">
+        <v>57.47</v>
+      </c>
+      <c r="I50">
         <v>63.35</v>
       </c>
-      <c r="H50">
+      <c r="J50">
+        <v>42.53</v>
+      </c>
+      <c r="K50">
         <v>36.42</v>
       </c>
-      <c r="I50">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="L50">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -1886,24 +2345,33 @@
         <v>83.28999999999999</v>
       </c>
       <c r="F51">
+        <v>0.17</v>
+      </c>
+      <c r="G51">
         <v>53.5</v>
       </c>
-      <c r="G51">
+      <c r="H51">
+        <v>64.23</v>
+      </c>
+      <c r="I51">
         <v>29.79</v>
       </c>
-      <c r="H51">
+      <c r="J51">
+        <v>35.77</v>
+      </c>
+      <c r="K51">
         <v>40.26</v>
       </c>
-      <c r="I51">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="L51">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C52">
         <v>7</v>
@@ -1915,24 +2383,33 @@
         <v>32.22</v>
       </c>
       <c r="F52">
+        <v>0.06</v>
+      </c>
+      <c r="G52">
         <v>21.67</v>
       </c>
-      <c r="G52">
+      <c r="H52">
+        <v>67.26000000000001</v>
+      </c>
+      <c r="I52">
         <v>10.55</v>
       </c>
-      <c r="H52">
+      <c r="J52">
+        <v>32.74</v>
+      </c>
+      <c r="K52">
         <v>46.01</v>
       </c>
-      <c r="I52">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="L52">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C53">
         <v>8</v>
@@ -1944,24 +2421,33 @@
         <v>34.62</v>
       </c>
       <c r="F53">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G53">
         <v>22.84</v>
       </c>
-      <c r="G53">
+      <c r="H53">
+        <v>65.97</v>
+      </c>
+      <c r="I53">
         <v>11.78</v>
       </c>
-      <c r="H53">
+      <c r="J53">
+        <v>34.03</v>
+      </c>
+      <c r="K53">
         <v>45.24</v>
       </c>
-      <c r="I53">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="L53">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C54">
         <v>4</v>
@@ -1973,24 +2459,33 @@
         <v>208.12</v>
       </c>
       <c r="F54">
+        <v>0.41</v>
+      </c>
+      <c r="G54">
         <v>107</v>
       </c>
-      <c r="G54">
+      <c r="H54">
+        <v>51.41</v>
+      </c>
+      <c r="I54">
         <v>101.12</v>
       </c>
-      <c r="H54">
+      <c r="J54">
+        <v>48.59</v>
+      </c>
+      <c r="K54">
         <v>30.2</v>
       </c>
-      <c r="I54">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="L54">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C55">
         <v>5</v>
@@ -2002,24 +2497,33 @@
         <v>344.55</v>
       </c>
       <c r="F55">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G55">
         <v>181.9</v>
       </c>
-      <c r="G55">
+      <c r="H55">
+        <v>52.79</v>
+      </c>
+      <c r="I55">
         <v>162.65</v>
       </c>
-      <c r="H55">
+      <c r="J55">
+        <v>47.21</v>
+      </c>
+      <c r="K55">
         <v>35.7</v>
       </c>
-      <c r="I55">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="L55">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -2031,24 +2535,33 @@
         <v>104.06</v>
       </c>
       <c r="F56">
+        <v>0.21</v>
+      </c>
+      <c r="G56">
         <v>53.5</v>
       </c>
-      <c r="G56">
+      <c r="H56">
+        <v>51.41</v>
+      </c>
+      <c r="I56">
         <v>50.56</v>
       </c>
-      <c r="H56">
+      <c r="J56">
+        <v>48.59</v>
+      </c>
+      <c r="K56">
         <v>38.19</v>
       </c>
-      <c r="I56">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="L56">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C57">
         <v>7</v>
@@ -2060,24 +2573,33 @@
         <v>253.37</v>
       </c>
       <c r="F57">
+        <v>0.5</v>
+      </c>
+      <c r="G57">
         <v>139.1</v>
       </c>
-      <c r="G57">
+      <c r="H57">
+        <v>54.9</v>
+      </c>
+      <c r="I57">
         <v>114.27</v>
       </c>
-      <c r="H57">
+      <c r="J57">
+        <v>45.1</v>
+      </c>
+      <c r="K57">
         <v>41.37</v>
       </c>
-      <c r="I57">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="L57">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C58">
         <v>8</v>
@@ -2089,24 +2611,33 @@
         <v>145.64</v>
       </c>
       <c r="F58">
+        <v>0.29</v>
+      </c>
+      <c r="G58">
         <v>75.14</v>
       </c>
-      <c r="G58">
+      <c r="H58">
+        <v>51.59</v>
+      </c>
+      <c r="I58">
         <v>70.5</v>
       </c>
-      <c r="H58">
+      <c r="J58">
+        <v>48.41</v>
+      </c>
+      <c r="K58">
         <v>43.98</v>
       </c>
-      <c r="I58">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="L58">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C59">
         <v>4</v>
@@ -2118,24 +2649,33 @@
         <v>19.49</v>
       </c>
       <c r="F59">
-        <v>10.7</v>
+        <v>0.04</v>
       </c>
       <c r="G59">
+        <v>10.7</v>
+      </c>
+      <c r="H59">
+        <v>54.9</v>
+      </c>
+      <c r="I59">
         <v>8.789999999999999</v>
       </c>
-      <c r="H59">
+      <c r="J59">
+        <v>45.1</v>
+      </c>
+      <c r="K59">
         <v>38.61</v>
       </c>
-      <c r="I59">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="L59">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C60">
         <v>5</v>
@@ -2147,24 +2687,33 @@
         <v>35.55</v>
       </c>
       <c r="F60">
-        <v>10.7</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G60">
+        <v>10.7</v>
+      </c>
+      <c r="H60">
+        <v>30.1</v>
+      </c>
+      <c r="I60">
         <v>24.85</v>
       </c>
-      <c r="H60">
+      <c r="J60">
+        <v>69.90000000000001</v>
+      </c>
+      <c r="K60">
         <v>45.82</v>
       </c>
-      <c r="I60">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="L60">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C61">
         <v>4</v>
@@ -2176,24 +2725,33 @@
         <v>39.45</v>
       </c>
       <c r="F61">
+        <v>0.08</v>
+      </c>
+      <c r="G61">
         <v>21.8</v>
       </c>
-      <c r="G61">
+      <c r="H61">
+        <v>55.26</v>
+      </c>
+      <c r="I61">
         <v>17.65</v>
       </c>
-      <c r="H61">
+      <c r="J61">
+        <v>44.74</v>
+      </c>
+      <c r="K61">
         <v>48.99</v>
       </c>
-      <c r="I61">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="L61">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C62">
         <v>5</v>
@@ -2205,24 +2763,33 @@
         <v>22.08</v>
       </c>
       <c r="F62">
+        <v>0.04</v>
+      </c>
+      <c r="G62">
         <v>12.93</v>
       </c>
-      <c r="G62">
+      <c r="H62">
+        <v>58.56</v>
+      </c>
+      <c r="I62">
         <v>9.15</v>
       </c>
-      <c r="H62">
+      <c r="J62">
+        <v>41.44</v>
+      </c>
+      <c r="K62">
         <v>49.01</v>
       </c>
-      <c r="I62">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="L62">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C63">
         <v>6</v>
@@ -2234,24 +2801,33 @@
         <v>27.11</v>
       </c>
       <c r="F63">
+        <v>0.05</v>
+      </c>
+      <c r="G63">
         <v>17.27</v>
       </c>
-      <c r="G63">
+      <c r="H63">
+        <v>63.7</v>
+      </c>
+      <c r="I63">
         <v>9.84</v>
       </c>
-      <c r="H63">
+      <c r="J63">
+        <v>36.3</v>
+      </c>
+      <c r="K63">
         <v>49.01</v>
       </c>
-      <c r="I63">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="L63">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C64">
         <v>7</v>
@@ -2263,24 +2839,33 @@
         <v>37.85</v>
       </c>
       <c r="F64">
+        <v>0.08</v>
+      </c>
+      <c r="G64">
         <v>20.83</v>
       </c>
-      <c r="G64">
+      <c r="H64">
+        <v>55.03</v>
+      </c>
+      <c r="I64">
         <v>17.02</v>
       </c>
-      <c r="H64">
+      <c r="J64">
+        <v>44.97</v>
+      </c>
+      <c r="K64">
         <v>49.01</v>
       </c>
-      <c r="I64">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="L64">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C65">
         <v>8</v>
@@ -2292,24 +2877,33 @@
         <v>32.38</v>
       </c>
       <c r="F65">
+        <v>0.06</v>
+      </c>
+      <c r="G65">
         <v>21.81</v>
       </c>
-      <c r="G65">
+      <c r="H65">
+        <v>67.36</v>
+      </c>
+      <c r="I65">
         <v>10.57</v>
       </c>
-      <c r="H65">
+      <c r="J65">
+        <v>32.64</v>
+      </c>
+      <c r="K65">
         <v>48.99</v>
       </c>
-      <c r="I65">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="L65">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C66">
         <v>3</v>
@@ -2321,24 +2915,33 @@
         <v>23.47</v>
       </c>
       <c r="F66">
+        <v>0.05</v>
+      </c>
+      <c r="G66">
         <v>14.13</v>
       </c>
-      <c r="G66">
+      <c r="H66">
+        <v>60.2</v>
+      </c>
+      <c r="I66">
         <v>9.34</v>
       </c>
-      <c r="H66">
+      <c r="J66">
+        <v>39.8</v>
+      </c>
+      <c r="K66">
         <v>51.99</v>
       </c>
-      <c r="I66">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="L66">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C67">
         <v>4</v>
@@ -2350,24 +2953,33 @@
         <v>38.98</v>
       </c>
       <c r="F67">
+        <v>0.08</v>
+      </c>
+      <c r="G67">
         <v>21.4</v>
       </c>
-      <c r="G67">
+      <c r="H67">
+        <v>54.9</v>
+      </c>
+      <c r="I67">
         <v>17.58</v>
       </c>
-      <c r="H67">
+      <c r="J67">
+        <v>45.1</v>
+      </c>
+      <c r="K67">
         <v>35.19</v>
       </c>
-      <c r="I67">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="L67">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C68">
         <v>5</v>
@@ -2379,24 +2991,33 @@
         <v>65.08</v>
       </c>
       <c r="F68">
+        <v>0.13</v>
+      </c>
+      <c r="G68">
         <v>32.09999999999999</v>
       </c>
-      <c r="G68">
+      <c r="H68">
+        <v>49.32</v>
+      </c>
+      <c r="I68">
         <v>32.98</v>
       </c>
-      <c r="H68">
+      <c r="J68">
+        <v>50.68</v>
+      </c>
+      <c r="K68">
         <v>40.26</v>
       </c>
-      <c r="I68">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="L68">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C69">
         <v>7</v>
@@ -2408,24 +3029,33 @@
         <v>59.11</v>
       </c>
       <c r="F69">
+        <v>0.12</v>
+      </c>
+      <c r="G69">
         <v>32.64</v>
       </c>
-      <c r="G69">
+      <c r="H69">
+        <v>55.22</v>
+      </c>
+      <c r="I69">
         <v>26.47</v>
       </c>
-      <c r="H69">
+      <c r="J69">
+        <v>44.78</v>
+      </c>
+      <c r="K69">
         <v>46.01</v>
       </c>
-      <c r="I69">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="L69">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C70">
         <v>8</v>
@@ -2437,24 +3067,33 @@
         <v>19.78</v>
       </c>
       <c r="F70">
+        <v>0.04</v>
+      </c>
+      <c r="G70">
         <v>10.95</v>
       </c>
-      <c r="G70">
+      <c r="H70">
+        <v>55.36</v>
+      </c>
+      <c r="I70">
         <v>8.83</v>
       </c>
-      <c r="H70">
+      <c r="J70">
+        <v>44.64</v>
+      </c>
+      <c r="K70">
         <v>45.98</v>
       </c>
-      <c r="I70">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="L70">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C71">
         <v>5</v>
@@ -2466,24 +3105,33 @@
         <v>25.78</v>
       </c>
       <c r="F71">
+        <v>0.05</v>
+      </c>
+      <c r="G71">
         <v>17.14</v>
       </c>
-      <c r="G71">
+      <c r="H71">
+        <v>66.48999999999999</v>
+      </c>
+      <c r="I71">
         <v>8.640000000000001</v>
       </c>
-      <c r="H71">
+      <c r="J71">
+        <v>33.51</v>
+      </c>
+      <c r="K71">
         <v>79.66</v>
       </c>
-      <c r="I71">
+      <c r="L71">
         <v>17.14</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C72">
         <v>2</v>
@@ -2495,24 +3143,33 @@
         <v>27.9</v>
       </c>
       <c r="F72">
+        <v>0.06</v>
+      </c>
+      <c r="G72">
         <v>19.9</v>
       </c>
-      <c r="G72">
+      <c r="H72">
+        <v>71.33</v>
+      </c>
+      <c r="I72">
         <v>8</v>
       </c>
-      <c r="H72">
+      <c r="J72">
+        <v>28.67</v>
+      </c>
+      <c r="K72">
         <v>74.38</v>
       </c>
-      <c r="I72">
+      <c r="L72">
         <v>9.949999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C73">
         <v>4</v>
@@ -2524,15 +3181,24 @@
         <v>112.53</v>
       </c>
       <c r="F73">
+        <v>0.22</v>
+      </c>
+      <c r="G73">
         <v>91.93000000000001</v>
       </c>
-      <c r="G73">
+      <c r="H73">
+        <v>81.69</v>
+      </c>
+      <c r="I73">
         <v>20.6</v>
       </c>
-      <c r="H73">
+      <c r="J73">
+        <v>18.31</v>
+      </c>
+      <c r="K73">
         <v>68</v>
       </c>
-      <c r="I73">
+      <c r="L73">
         <v>9.949999999999999</v>
       </c>
     </row>

</xml_diff>